<commit_message>
Update pattern 29 Dec
</commit_message>
<xml_diff>
--- a/pattern_leetcode.xlsx
+++ b/pattern_leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software\Leetcode-Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FB83C7-5712-40DB-9624-A1C1B043C7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1E1E64-B1E4-417C-AF35-3083065856DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="741" xr2:uid="{DE4D0EC4-9EBA-4342-877D-CEAD3830BD96}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="203">
   <si>
     <t>Pattern</t>
   </si>
@@ -1026,7 +1026,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-14009]dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -1138,13 +1138,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1567,7 +1567,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1725,8 +1725,12 @@
       <c r="C9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="15">
+        <v>45655</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="5" t="s">
@@ -1738,8 +1742,12 @@
       <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="15">
+        <v>45655</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="30">
       <c r="A11" s="5" t="s">
@@ -1798,7 +1806,7 @@
       <c r="E14" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D14 E1">
+  <conditionalFormatting sqref="E1 A1:D14">
     <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
@@ -1896,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B3ED86-AF96-4E07-A077-3E1EFBACAA2C}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2146,7 +2154,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>